<commit_message>
fix: use existing json_to_excel_fixture.py instead of custom generator
- Remove unnecessary json_to_sheet_context_fixture.py
- Modify sheet_context_test_cases.json to match json_to_excel_fixture.py format
- Use established data_sheet, auxiliary_data, and levels structure
- Regenerate sheet_context_test.xlsx with proper Tests sheet structure
- Add README_SHEET_CONTEXT.md documenting the correct approach
- Maintain backward compatibility with integration tests (3 tests pass)
- Follow DRY principle: reuse existing infrastructure instead of duplicating

Benefits:
- Eliminates code duplication
- Uses proven json_to_excel_fixture.py infrastructure
- Consistent with other test generators in resources_generator
- Maintainable JSON-driven configuration
- Clear documentation of proper usage

Co-authored-by: Ona <no-reply@ona.com>
</commit_message>
<xml_diff>
--- a/tests/resources/sheet_context_test.xlsx
+++ b/tests/resources/sheet_context_test.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Tests" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -516,4 +517,59 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1">
+        <f>Sheet1!C1</f>
+        <v/>
+      </c>
+      <c r="B1">
+        <f>Sheet1!C2</f>
+        <v/>
+      </c>
+      <c r="C1">
+        <f>Sheet1!D1</f>
+        <v/>
+      </c>
+      <c r="D1">
+        <f>Sheet1!A1</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <f>Sheet2!C1</f>
+        <v/>
+      </c>
+      <c r="B2">
+        <f>Sheet2!C2</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>Sheet2!D1</f>
+        <v/>
+      </c>
+      <c r="D2">
+        <f>Sheet2!A1</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>